<commit_message>
EPBDS-9385 Update error messages for tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9385_Uppercase_validation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9385_Uppercase_validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpushko/EIS/1. EPBDS/EPBDS-9385/sent for review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE74A02-EA2C-F14F-BD06-1EDC744279AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD1060-61EA-114D-BC15-B6F5383A5432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2000" windowWidth="19100" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="1060" windowWidth="20460" windowHeight="13100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
   <si>
     <t xml:space="preserve">Datatype MyDatatype </t>
   </si>
@@ -676,33 +676,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1089,18 +1089,18 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="E4" s="22" t="s">
+      <c r="C4" s="23"/>
+      <c r="E4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="I4" s="20" t="s">
+      <c r="F4" s="24"/>
+      <c r="I4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1176,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:G38"/>
+  <dimension ref="B3:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1197,11 +1197,11 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
@@ -1262,53 +1262,37 @@
         <v>22</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>52</v>
-      </c>
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
@@ -1318,91 +1302,107 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="E15" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
+      <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>62</v>
+      <c r="E20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>51</v>
+      <c r="E21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>46</v>
+      <c r="E22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
@@ -1413,154 +1413,90 @@
         <v>22</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="E27" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="E30" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="E28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E35" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E36" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E37" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E38" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F38" s="10" t="s">
+      <c r="F32" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G32" s="11" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1584,13 +1520,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="C4" s="25"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
@@ -1713,7 +1649,7 @@
       <c r="E20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="20" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1757,7 +1693,7 @@
       <c r="E26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="20" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>